<commit_message>
Updated performance matrix list 04/20/2021
</commit_message>
<xml_diff>
--- a/Deliverables/Model_Experiemental_Results.xlsx
+++ b/Deliverables/Model_Experiemental_Results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/soumavadey/Documents/CS598_DLH/final project/GitHub/COVID-19-CHEST-X-RAY-IMAGE-CLASSISICATION/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/soumavadey/Documents/CS598_DLH/final project/GitHub/COVID-19-CHEST-X-RAY-IMAGE-CLASSISICATION/Deliverables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80D07662-5F02-754E-BC55-4C7C1AEC41EF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{817561EA-7E8E-524A-B6A3-C5305C0F4220}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15840" activeTab="3" xr2:uid="{5372D0ED-CE0A-944B-84C9-250E41CD4459}"/>
+    <workbookView xWindow="-480" yWindow="5940" windowWidth="28800" windowHeight="15840" activeTab="3" xr2:uid="{5372D0ED-CE0A-944B-84C9-250E41CD4459}"/>
   </bookViews>
   <sheets>
     <sheet name="Arjun" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
   <si>
     <t>Model</t>
   </si>
@@ -46,13 +46,76 @@
   </si>
   <si>
     <t>Parameters(Optimizer, Learning Rate, Epochs)</t>
+  </si>
+  <si>
+    <t>ResNet50</t>
+  </si>
+  <si>
+    <t>Imagesize</t>
+  </si>
+  <si>
+    <t>Centercrop</t>
+  </si>
+  <si>
+    <t>normalization</t>
+  </si>
+  <si>
+    <t>Optimizer</t>
+  </si>
+  <si>
+    <t>Learning Rate</t>
+  </si>
+  <si>
+    <t>Dataset</t>
+  </si>
+  <si>
+    <t>Train</t>
+  </si>
+  <si>
+    <t>Validation</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>SGD</t>
+  </si>
+  <si>
+    <t>Parameters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accuracy </t>
+  </si>
+  <si>
+    <t>Precision</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Recall</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> F1-score</t>
+  </si>
+  <si>
+    <t>Validation Measures</t>
+  </si>
+  <si>
+    <t>ResNet101</t>
+  </si>
+  <si>
+    <t>Epoch</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.E+00"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -68,6 +131,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF212121"/>
+      <name val="Courier New"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -77,7 +146,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -85,16 +154,52 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -525,26 +630,230 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83D16FEE-4981-2243-9476-FEDF3EECD13F}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="4" width="20.5" customWidth="1"/>
+    <col min="5" max="5" width="19.6640625" customWidth="1"/>
+    <col min="6" max="6" width="17.5" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" customWidth="1"/>
+    <col min="8" max="8" width="15.5" customWidth="1"/>
+    <col min="9" max="9" width="20.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="B1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2" s="7"/>
+      <c r="B2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="9">
+        <v>70</v>
+      </c>
+      <c r="C3" s="9">
+        <v>15</v>
+      </c>
+      <c r="D3" s="9">
+        <v>15</v>
+      </c>
+      <c r="E3" s="9">
+        <v>224</v>
+      </c>
+      <c r="F3" s="9">
+        <v>200</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="10">
+        <v>0.01</v>
+      </c>
+      <c r="J3" s="9">
+        <v>25</v>
+      </c>
+      <c r="K3" s="9">
+        <v>0.93146399999999996</v>
+      </c>
+      <c r="L3" s="9">
+        <v>0.91048899999999999</v>
+      </c>
+      <c r="M3" s="9">
+        <v>0.91822700000000002</v>
+      </c>
+      <c r="N3" s="9">
+        <v>0.91416900000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="9">
+        <v>70</v>
+      </c>
+      <c r="C4" s="9">
+        <v>15</v>
+      </c>
+      <c r="D4" s="9">
+        <v>15</v>
+      </c>
+      <c r="E4" s="9">
+        <v>224</v>
+      </c>
+      <c r="F4" s="9">
+        <v>224</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" s="10">
+        <v>0.01</v>
+      </c>
+      <c r="J4" s="9">
+        <v>25</v>
+      </c>
+      <c r="K4" s="9">
+        <v>0.93561799999999995</v>
+      </c>
+      <c r="L4" s="9">
+        <v>0.91192300000000004</v>
+      </c>
+      <c r="M4" s="9">
+        <v>0.93480399999999997</v>
+      </c>
+      <c r="N4" s="9">
+        <v>0.92291800000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="9">
+        <v>70</v>
+      </c>
+      <c r="C5" s="9">
+        <v>15</v>
+      </c>
+      <c r="D5" s="9">
+        <v>15</v>
+      </c>
+      <c r="E5" s="9">
+        <v>224</v>
+      </c>
+      <c r="F5" s="9">
+        <v>224</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" s="10">
+        <v>0.01</v>
+      </c>
+      <c r="J5" s="9">
+        <v>25</v>
+      </c>
+      <c r="K5" s="9">
+        <v>0.93665600000000004</v>
+      </c>
+      <c r="L5" s="9">
+        <v>0.94180600000000003</v>
+      </c>
+      <c r="M5" s="9">
+        <v>0.91849800000000004</v>
+      </c>
+      <c r="N5" s="9">
+        <v>0.92884699999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+      <c r="K6" s="8"/>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:J1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="K1:N1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add experimental results SAM 04/21/2021
</commit_message>
<xml_diff>
--- a/Deliverables/Model_Experiemental_Results.xlsx
+++ b/Deliverables/Model_Experiemental_Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/soumavadey/Documents/CS598_DLH/final project/GitHub/COVID-19-CHEST-X-RAY-IMAGE-CLASSISICATION/Deliverables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{817561EA-7E8E-524A-B6A3-C5305C0F4220}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5D476C50-738E-F04E-B204-4CC6E111A26D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-480" yWindow="5940" windowWidth="28800" windowHeight="15840" activeTab="3" xr2:uid="{5372D0ED-CE0A-944B-84C9-250E41CD4459}"/>
+    <workbookView xWindow="0" yWindow="1660" windowWidth="28800" windowHeight="15840" activeTab="3" xr2:uid="{5372D0ED-CE0A-944B-84C9-250E41CD4459}"/>
   </bookViews>
   <sheets>
     <sheet name="Arjun" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="23">
   <si>
     <t>Model</t>
   </si>
@@ -115,7 +115,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.E+00"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -130,12 +130,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FF212121"/>
-      <name val="Courier New"/>
-      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -173,12 +167,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -186,19 +192,10 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -630,10 +627,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83D16FEE-4981-2243-9476-FEDF3EECD13F}">
-  <dimension ref="A1:N6"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -647,205 +644,422 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="3" t="s">
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="3" t="s">
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A2" s="7"/>
-      <c r="B2" s="5" t="s">
+      <c r="A2" s="12"/>
+      <c r="B2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="K2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="L2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="M2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="N2" s="3" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B3" s="4">
         <v>70</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="4">
         <v>15</v>
       </c>
-      <c r="D3" s="9">
+      <c r="D3" s="4">
         <v>15</v>
       </c>
-      <c r="E3" s="9">
-        <v>224</v>
-      </c>
-      <c r="F3" s="9">
+      <c r="E3" s="4">
+        <v>224</v>
+      </c>
+      <c r="F3" s="4">
         <v>200</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="H3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="10">
+      <c r="I3" s="5">
         <v>0.01</v>
       </c>
-      <c r="J3" s="9">
+      <c r="J3" s="4">
         <v>25</v>
       </c>
-      <c r="K3" s="9">
+      <c r="K3" s="4">
         <v>0.93146399999999996</v>
       </c>
-      <c r="L3" s="9">
+      <c r="L3" s="4">
         <v>0.91048899999999999</v>
       </c>
-      <c r="M3" s="9">
+      <c r="M3" s="4">
         <v>0.91822700000000002</v>
       </c>
-      <c r="N3" s="9">
+      <c r="N3" s="4">
         <v>0.91416900000000001</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="4">
         <v>70</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="4">
         <v>15</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="4">
         <v>15</v>
       </c>
-      <c r="E4" s="9">
-        <v>224</v>
-      </c>
-      <c r="F4" s="9">
-        <v>224</v>
-      </c>
-      <c r="G4" s="9" t="s">
+      <c r="E4" s="4">
+        <v>224</v>
+      </c>
+      <c r="F4" s="4">
+        <v>224</v>
+      </c>
+      <c r="G4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="H4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="10">
+      <c r="I4" s="5">
         <v>0.01</v>
       </c>
-      <c r="J4" s="9">
+      <c r="J4" s="4">
         <v>25</v>
       </c>
-      <c r="K4" s="9">
+      <c r="K4" s="4">
         <v>0.93561799999999995</v>
       </c>
-      <c r="L4" s="9">
+      <c r="L4" s="4">
         <v>0.91192300000000004</v>
       </c>
-      <c r="M4" s="9">
+      <c r="M4" s="4">
         <v>0.93480399999999997</v>
       </c>
-      <c r="N4" s="9">
+      <c r="N4" s="4">
         <v>0.92291800000000002</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5" s="4">
         <v>70</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="4">
         <v>15</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="4">
         <v>15</v>
       </c>
-      <c r="E5" s="9">
-        <v>224</v>
-      </c>
-      <c r="F5" s="9">
-        <v>224</v>
-      </c>
-      <c r="G5" s="9" t="s">
+      <c r="E5" s="4">
+        <v>224</v>
+      </c>
+      <c r="F5" s="4">
+        <v>224</v>
+      </c>
+      <c r="G5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="9" t="s">
+      <c r="H5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="10">
+      <c r="I5" s="5">
         <v>0.01</v>
       </c>
-      <c r="J5" s="9">
+      <c r="J5" s="4">
         <v>25</v>
       </c>
-      <c r="K5" s="9">
+      <c r="K5" s="4">
         <v>0.93665600000000004</v>
       </c>
-      <c r="L5" s="9">
+      <c r="L5" s="4">
         <v>0.94180600000000003</v>
       </c>
-      <c r="M5" s="9">
+      <c r="M5" s="4">
         <v>0.91849800000000004</v>
       </c>
-      <c r="N5" s="9">
+      <c r="N5" s="4">
         <v>0.92884699999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="19" x14ac:dyDescent="0.25">
-      <c r="K6" s="8"/>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="4">
+        <v>70</v>
+      </c>
+      <c r="C6" s="4">
+        <v>15</v>
+      </c>
+      <c r="D6" s="4">
+        <v>15</v>
+      </c>
+      <c r="E6" s="4">
+        <v>224</v>
+      </c>
+      <c r="F6" s="4">
+        <v>224</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="J6" s="7">
+        <v>50</v>
+      </c>
+      <c r="K6" s="4">
+        <v>0.94392500000000001</v>
+      </c>
+      <c r="L6" s="4">
+        <v>0.94566600000000001</v>
+      </c>
+      <c r="M6" s="4">
+        <v>0.93929399999999996</v>
+      </c>
+      <c r="N6" s="4">
+        <v>0.94203700000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="4">
+        <v>80</v>
+      </c>
+      <c r="C7" s="4">
+        <v>10</v>
+      </c>
+      <c r="D7" s="4">
+        <v>10</v>
+      </c>
+      <c r="E7" s="4">
+        <v>224</v>
+      </c>
+      <c r="F7" s="4">
+        <v>224</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="J7" s="7">
+        <v>25</v>
+      </c>
+      <c r="K7" s="4">
+        <v>0.93488400000000005</v>
+      </c>
+      <c r="L7" s="4">
+        <v>0.94355900000000004</v>
+      </c>
+      <c r="M7" s="4">
+        <v>0.90717499999999995</v>
+      </c>
+      <c r="N7" s="4">
+        <v>0.92432700000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="4">
+        <v>80</v>
+      </c>
+      <c r="C8" s="4">
+        <v>10</v>
+      </c>
+      <c r="D8" s="4">
+        <v>10</v>
+      </c>
+      <c r="E8" s="4">
+        <v>224</v>
+      </c>
+      <c r="F8" s="4">
+        <v>224</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="J8" s="7">
+        <v>25</v>
+      </c>
+      <c r="K8" s="4">
+        <v>0.922481</v>
+      </c>
+      <c r="L8" s="4">
+        <v>0.92986199999999997</v>
+      </c>
+      <c r="M8" s="4">
+        <v>0.885737</v>
+      </c>
+      <c r="N8" s="4">
+        <v>0.90622199999999997</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="4">
+        <v>80</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0</v>
+      </c>
+      <c r="D9" s="4">
+        <v>20</v>
+      </c>
+      <c r="E9" s="4">
+        <v>224</v>
+      </c>
+      <c r="F9" s="4">
+        <v>224</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I9" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="J9" s="7">
+        <v>25</v>
+      </c>
+      <c r="K9" s="4">
+        <v>0.93167699999999998</v>
+      </c>
+      <c r="L9" s="4">
+        <v>0.93730599999999997</v>
+      </c>
+      <c r="M9" s="4">
+        <v>0.90793500000000005</v>
+      </c>
+      <c r="N9" s="4">
+        <v>0.921933</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="4">
+        <v>80</v>
+      </c>
+      <c r="C10" s="4">
+        <v>0</v>
+      </c>
+      <c r="D10" s="4">
+        <v>20</v>
+      </c>
+      <c r="E10" s="4">
+        <v>224</v>
+      </c>
+      <c r="F10" s="4">
+        <v>224</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I10" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="J10" s="7">
+        <v>25</v>
+      </c>
+      <c r="K10" s="4">
+        <v>0.93788800000000005</v>
+      </c>
+      <c r="L10" s="4">
+        <v>0.93720700000000001</v>
+      </c>
+      <c r="M10" s="4">
+        <v>0.92809399999999997</v>
+      </c>
+      <c r="N10" s="4">
+        <v>0.93167800000000001</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -855,5 +1069,6 @@
     <mergeCell ref="K1:N1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>